<commit_message>
añadir tipo de error en sección 1, finalización sistema y radio sor
</commit_message>
<xml_diff>
--- a/app/tables/tabla_biseccion.xlsx
+++ b/app/tables/tabla_biseccion.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -495,7 +495,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>2.5</t>
+          <t>1.0</t>
         </is>
       </c>
     </row>
@@ -517,7 +517,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>1.25</t>
+          <t>0.333333333333333</t>
         </is>
       </c>
     </row>
@@ -539,7 +539,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>0.625</t>
+          <t>0.2</t>
         </is>
       </c>
     </row>
@@ -561,7 +561,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>0.3125</t>
+          <t>0.0909090909090909</t>
         </is>
       </c>
     </row>
@@ -583,7 +583,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>0.15625</t>
+          <t>0.0476190476190476</t>
         </is>
       </c>
     </row>
@@ -605,7 +605,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>0.078125</t>
+          <t>0.024390243902439</t>
         </is>
       </c>
     </row>
@@ -627,7 +627,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>0.0390625</t>
+          <t>0.0123456790123457</t>
         </is>
       </c>
     </row>
@@ -649,7 +649,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>0.01953125</t>
+          <t>0.0061349693251533</t>
         </is>
       </c>
     </row>
@@ -671,7 +671,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>0.009765625</t>
+          <t>0.003076923076923</t>
         </is>
       </c>
     </row>
@@ -693,7 +693,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>0.0048828125</t>
+          <t>0.0015408320493066</t>
         </is>
       </c>
     </row>
@@ -715,7 +715,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>0.00244140625</t>
+          <t>0.0007710100231303</t>
         </is>
       </c>
     </row>
@@ -737,7 +737,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>0.001220703125</t>
+          <t>0.0003856536829926</t>
         </is>
       </c>
     </row>
@@ -759,7 +759,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>0.0006103515625</t>
+          <t>0.0001928640308582</t>
         </is>
       </c>
     </row>
@@ -781,7 +781,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>0.00030517578125</t>
+          <t>9.64413154595429e-05</t>
         </is>
       </c>
     </row>
@@ -803,7 +803,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>0.000152587890625</t>
+          <t>4.82229830737329e-05</t>
         </is>
       </c>
     </row>
@@ -825,7 +825,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>7.62939453125e-05</t>
+          <t>2.41109101868596e-05</t>
         </is>
       </c>
     </row>
@@ -847,7 +847,7 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>3.814697265625e-05</t>
+          <t>1.20556004291794e-05</t>
         </is>
       </c>
     </row>
@@ -869,7 +869,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>1.9073486328125e-05</t>
+          <t>6.02783654918413e-06</t>
         </is>
       </c>
     </row>
@@ -891,29 +891,7 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>9.5367431640625e-06</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>20</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>-3.1642484664917</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>2.51429654994448e-05</t>
-        </is>
-      </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>4.76837158203125e-06</t>
+          <t>3.01390919091608e-06</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
nombres de variables más descriptivos sección 1 y 2, y valor de w 0<w<2
</commit_message>
<xml_diff>
--- a/app/tables/tabla_biseccion.xlsx
+++ b/app/tables/tabla_biseccion.xlsx
@@ -463,12 +463,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>17.5</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>-11.0</t>
+          <t>-15.5354061665063</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -485,17 +485,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>-2.5</t>
+          <t>28.75</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>-3.78125</t>
+          <t>-7.76046437070352</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>2.5</t>
+          <t>11.25</t>
         </is>
       </c>
     </row>
@@ -507,17 +507,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>-3.75</t>
+          <t>34.375</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>4.05697572827198</t>
+          <t>-3.38630689190715</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>1.25</t>
+          <t>5.625</t>
         </is>
       </c>
     </row>
@@ -529,17 +529,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>-3.125</t>
+          <t>37.1875</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>-0.247514006488339</t>
+          <t>-1.12430878314094</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>0.625</t>
+          <t>2.8125</t>
         </is>
       </c>
     </row>
@@ -551,17 +551,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>-3.4375</t>
+          <t>38.59375</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>1.80788665833855</t>
+          <t>0.022117576163545</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>0.3125</t>
+          <t>1.40625</t>
         </is>
       </c>
     </row>
@@ -573,17 +573,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>-3.28125</t>
+          <t>37.890625</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>0.756021441039556</t>
+          <t>-0.552301040083382</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>0.15625</t>
+          <t>0.703125</t>
         </is>
       </c>
     </row>
@@ -595,17 +595,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>-3.203125</t>
+          <t>38.2421875</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>0.248219418534426</t>
+          <t>-0.265387537314954</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>0.078125</t>
+          <t>0.3515625</t>
         </is>
       </c>
     </row>
@@ -617,17 +617,17 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>-3.1640625</t>
+          <t>38.41796875</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>-0.0011549191511122</t>
+          <t>-0.121708254405178</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>0.0390625</t>
+          <t>0.17578125</t>
         </is>
       </c>
     </row>
@@ -639,17 +639,17 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>-3.18359375</t>
+          <t>38.505859375</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>0.123155220682149</t>
+          <t>-0.0498135739055385</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>0.01953125</t>
+          <t>0.087890625</t>
         </is>
       </c>
     </row>
@@ -661,17 +661,17 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>-3.173828125</t>
+          <t>38.5498046875</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>0.0609059085934192</t>
+          <t>-0.0138525471707283</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>0.009765625</t>
+          <t>0.0439453125</t>
         </is>
       </c>
     </row>
@@ -683,17 +683,17 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>-3.1689453125</t>
+          <t>38.57177734375</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>0.0298519360855689</t>
+          <t>0.0041313787171439</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>0.0048828125</t>
+          <t>0.02197265625</t>
         </is>
       </c>
     </row>
@@ -705,17 +705,17 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>-3.16650390625</t>
+          <t>38.560791015625</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>0.0143426190481772</t>
+          <t>-0.0048608683333952</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>0.00244140625</t>
+          <t>0.010986328125</t>
         </is>
       </c>
     </row>
@@ -727,17 +727,17 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>-3.165283203125</t>
+          <t>38.5662841796875</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>0.0065923776238392</t>
+          <t>-0.0003648158145423</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>0.001220703125</t>
+          <t>0.0054931640625</t>
         </is>
       </c>
     </row>
@@ -749,17 +749,17 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>-3.1646728515625</t>
+          <t>38.5690307617188</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>0.0027183611589549</t>
+          <t>0.0018832637022256</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>0.0006103515625</t>
+          <t>0.00274658203125</t>
         </is>
       </c>
     </row>
@@ -771,17 +771,17 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>-3.16436767578125</t>
+          <t>38.5676574707031</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>0.0007816289850399</t>
+          <t>0.0007592195062571</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>0.00030517578125</t>
+          <t>0.001373291015625</t>
         </is>
       </c>
     </row>
@@ -793,17 +793,17 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>-3.16421508789062</t>
+          <t>38.5669708251953</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>-0.0001866680876965</t>
+          <t>0.000197200736423</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>0.000152587890625</t>
+          <t>0.0006866455078125</t>
         </is>
       </c>
     </row>
@@ -815,17 +815,17 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>-3.16429138183594</t>
+          <t>38.5666275024414</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>0.0002974746974988</t>
+          <t>-8.38078164235867e-05</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>7.62939453125e-05</t>
+          <t>0.0003433227539062</t>
         </is>
       </c>
     </row>
@@ -837,17 +837,17 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>-3.16425323486328</t>
+          <t>38.5667991638184</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>5.54018671081735e-05</t>
+          <t>5.66963906578621e-05</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>3.814697265625e-05</t>
+          <t>0.0001716613769531</t>
         </is>
       </c>
     </row>
@@ -859,17 +859,17 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>-3.16423416137695</t>
+          <t>38.5667133331299</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>-6.56334697417549e-05</t>
+          <t>-1.35557302165523e-05</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>1.9073486328125e-05</t>
+          <t>8.58306884765625e-05</t>
         </is>
       </c>
     </row>
@@ -881,17 +881,17 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>-3.16424369812012</t>
+          <t>38.5667562484741</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>-5.11589117913047e-06</t>
+          <t>2.15703258845679e-05</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>9.5367431640625e-06</t>
+          <t>4.29153442382812e-05</t>
         </is>
       </c>
     </row>
@@ -903,17 +903,17 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>-3.1642484664917</t>
+          <t>38.566734790802</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>2.51429654998248e-05</t>
+          <t>4.00729675220646e-06</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>4.76837158203125e-06</t>
+          <t>2.14576721191406e-05</t>
         </is>
       </c>
     </row>

</xml_diff>